<commit_message>
update for insert release-notes.md f80ed2bb9e1dd81abc71d13817b8a44a756cee80
</commit_message>
<xml_diff>
--- a/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.0</t>
+    <t>0.4.0-snapshot-1</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>active</t>
+    <t>draft</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-13T09:33:00+00:00</t>
+    <t>2024-05-23T12:16:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -66,7 +66,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>ANS (https://esante.gouv.fr)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>